<commit_message>
working on student template uploader
</commit_message>
<xml_diff>
--- a/public/templates/Student template.xlsx
+++ b/public/templates/Student template.xlsx
@@ -287,7 +287,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="38">
   <si>
     <t>No</t>
   </si>
@@ -389,6 +389,18 @@
   </si>
   <si>
     <t>entah2@entah.com7</t>
+  </si>
+  <si>
+    <t>XXXX</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>kljlj</t>
   </si>
 </sst>
 </file>
@@ -722,7 +734,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +880,7 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -938,7 +950,7 @@
         <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -973,7 +985,7 @@
         <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
         <v>18</v>
@@ -981,8 +993,8 @@
       <c r="J7" t="s">
         <v>19</v>
       </c>
-      <c r="K7">
-        <v>2025</v>
+      <c r="K7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changing template, responsive improvement, add find invoice button to menubar, etc
</commit_message>
<xml_diff>
--- a/public/templates/Student template.xlsx
+++ b/public/templates/Student template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -258,36 +258,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>SERVER3:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Panjang Tahun masuk maksimal 4 karakter angka dan wajib diisi</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="34">
   <si>
     <t>No</t>
   </si>
@@ -319,9 +295,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Tahun masuk</t>
-  </si>
-  <si>
     <t>2021.x.21</t>
   </si>
   <si>
@@ -391,16 +364,7 @@
     <t>entah2@entah.com7</t>
   </si>
   <si>
-    <t>XXXX</t>
-  </si>
-  <si>
     <t>BS</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>kljlj</t>
   </si>
 </sst>
 </file>
@@ -731,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,10 +713,9 @@
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -783,288 +746,261 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2">
-        <v>2020</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3">
-        <v>2021</v>
-      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4">
-        <v>2022</v>
-      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5">
-        <v>2023</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
-        <v>36</v>
-      </c>
       <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
         <v>18</v>
       </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6">
-        <v>2024</v>
-      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" t="s">
-        <v>37</v>
-      </c>
       <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
         <v>18</v>
       </c>
-      <c r="J7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>18</v>
       </c>
-      <c r="J8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8">
-        <v>2026</v>
-      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>15</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>16</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>17</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>18</v>
-      </c>
-      <c r="J9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9">
-        <v>2027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>